<commit_message>
Fixed naming issue and generated landing figures
</commit_message>
<xml_diff>
--- a/crazyflie_projects/DeepRL/Angled_Surface_Data_Collection.xlsx
+++ b/crazyflie_projects/DeepRL/Angled_Surface_Data_Collection.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="20">
   <si>
     <t xml:space="preserve">Leg Config</t>
   </si>
@@ -52,19 +52,22 @@
     <t xml:space="preserve">[ -90 – 45 ]</t>
   </si>
   <si>
+    <t xml:space="preserve">X</t>
+  </si>
+  <si>
     <t xml:space="preserve">[ -90 – 90 ]</t>
   </si>
   <si>
     <t xml:space="preserve">[ -45 – 90 ]</t>
   </si>
   <si>
+    <t xml:space="preserve">-</t>
+  </si>
+  <si>
     <t xml:space="preserve">[   0 – 90 ]</t>
   </si>
   <si>
     <t xml:space="preserve">A30_L75_K32</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X</t>
   </si>
   <si>
     <t xml:space="preserve">A60_L75_K32</t>
@@ -228,7 +231,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -312,10 +315,10 @@
   <dimension ref="A1:AMJ31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.61"/>
@@ -385,13 +388,17 @@
       <c r="B4" s="4" t="n">
         <v>90</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
+      <c r="C4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="E4" s="4" t="s">
         <v>7</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -401,13 +408,17 @@
       <c r="B5" s="4" t="n">
         <v>135</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
+      <c r="C5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="E5" s="4" t="s">
         <v>7</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -417,24 +428,32 @@
       <c r="B6" s="4" t="n">
         <v>180</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
+      <c r="C6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>13</v>
+      </c>
       <c r="E6" s="4" t="s">
         <v>7</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B7" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
+      <c r="C7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>10</v>
+      </c>
       <c r="E7" s="6" t="s">
         <v>7</v>
       </c>
@@ -444,13 +463,17 @@
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B8" s="6" t="n">
         <v>45</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
+      <c r="C8" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>10</v>
+      </c>
       <c r="E8" s="6" t="s">
         <v>7</v>
       </c>
@@ -460,57 +483,67 @@
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B9" s="6" t="n">
         <v>90</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="7"/>
+        <v>10</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>10</v>
+      </c>
       <c r="E9" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B10" s="6" t="n">
         <v>135</v>
       </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
+      <c r="C10" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>10</v>
+      </c>
       <c r="E10" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B11" s="6" t="n">
         <v>180</v>
       </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
+      <c r="C11" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>10</v>
+      </c>
       <c r="E11" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B12" s="4" t="n">
         <v>0</v>
@@ -526,7 +559,7 @@
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B13" s="4" t="n">
         <v>45</v>
@@ -542,7 +575,7 @@
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B14" s="4" t="n">
         <v>90</v>
@@ -553,12 +586,12 @@
         <v>7</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B15" s="4" t="n">
         <v>135</v>
@@ -569,12 +602,12 @@
         <v>7</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B16" s="4" t="n">
         <v>180</v>
@@ -585,12 +618,12 @@
         <v>7</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B17" s="6" t="n">
         <v>0</v>
@@ -606,7 +639,7 @@
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B18" s="6" t="n">
         <v>45</v>
@@ -622,7 +655,7 @@
     </row>
     <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B19" s="6" t="n">
         <v>90</v>
@@ -633,12 +666,12 @@
         <v>7</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B20" s="6" t="n">
         <v>135</v>
@@ -649,12 +682,12 @@
         <v>7</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B21" s="6" t="n">
         <v>180</v>
@@ -665,12 +698,12 @@
         <v>7</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B22" s="4" t="n">
         <v>0</v>
@@ -686,7 +719,7 @@
     </row>
     <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B23" s="4" t="n">
         <v>45</v>
@@ -702,7 +735,7 @@
     </row>
     <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B24" s="4" t="n">
         <v>90</v>
@@ -713,12 +746,12 @@
         <v>7</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B25" s="4" t="n">
         <v>135</v>
@@ -729,12 +762,12 @@
         <v>7</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B26" s="4" t="n">
         <v>180</v>
@@ -745,12 +778,12 @@
         <v>7</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B27" s="6" t="n">
         <v>0</v>
@@ -766,7 +799,7 @@
     </row>
     <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B28" s="6" t="n">
         <v>45</v>
@@ -782,7 +815,7 @@
     </row>
     <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B29" s="6" t="n">
         <v>90</v>
@@ -793,12 +826,12 @@
         <v>7</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B30" s="6" t="n">
         <v>135</v>
@@ -809,12 +842,12 @@
         <v>7</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B31" s="6" t="n">
         <v>180</v>
@@ -825,7 +858,7 @@
         <v>7</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>